<commit_message>
Data clean and almost prepared for correlation analysis
</commit_message>
<xml_diff>
--- a/5_Traits.xlsx
+++ b/5_Traits.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="203">
   <si>
     <t>Horodateur</t>
   </si>
@@ -584,6 +584,42 @@
   </si>
   <si>
     <t>Ithan</t>
+  </si>
+  <si>
+    <t>alize.bosio@insa-lyon.fr</t>
+  </si>
+  <si>
+    <t>Bosio</t>
+  </si>
+  <si>
+    <t>Alizé</t>
+  </si>
+  <si>
+    <t>mariana.escobar-quiceno@enise.fr</t>
+  </si>
+  <si>
+    <t>Escobar Quiceno</t>
+  </si>
+  <si>
+    <t>Mariana</t>
+  </si>
+  <si>
+    <t>charles.riotte03@gmail.com</t>
+  </si>
+  <si>
+    <t>Riotte</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>rany.ward@insa-lyon.fr</t>
+  </si>
+  <si>
+    <t>Ward</t>
+  </si>
+  <si>
+    <t>Rany</t>
   </si>
 </sst>
 </file>
@@ -593,7 +629,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -601,6 +637,9 @@
     </font>
     <font>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -618,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -648,6 +687,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1083,28 +1125,28 @@
         <v>6.0</v>
       </c>
       <c r="AJ2" s="7">
-        <f t="shared" ref="AJ2:AJ52" si="1">ROUND(SUM(J2,8-K2,8-L2,M2,N2,-5) /30 * 100,0)</f>
+        <f t="shared" ref="AJ2:AJ57" si="1">ROUND(SUM(J2,8-K2,8-L2,M2,N2,-5) /30 * 100,0)</f>
         <v>90</v>
       </c>
       <c r="AK2" s="7">
-        <f t="shared" ref="AK2:AK52" si="2">ROUND(SUM(O2,P2,Q2,R2,S2-5)/30 * 100,0)</f>
+        <f t="shared" ref="AK2:AK57" si="2">ROUND(SUM(O2,P2,Q2,R2,S2-5)/30 * 100,0)</f>
         <v>77</v>
       </c>
       <c r="AL2" s="7">
-        <f t="shared" ref="AL2:AL52" si="3">ROUND(SUM(T2,U2,(8-V2),(8-W2),(8-X2)-5)/30 * 100,0)</f>
+        <f t="shared" ref="AL2:AL57" si="3">ROUND(SUM(T2,U2,(8-V2),(8-W2),(8-X2)-5)/30 * 100,0)</f>
         <v>77</v>
       </c>
       <c r="AM2" s="7">
-        <f t="shared" ref="AM2:AM52" si="4">ROUND(SUM(Y2,Z2,AA2,AB2,AC2-5)/30 * 100,0)</f>
+        <f t="shared" ref="AM2:AM57" si="4">ROUND(SUM(Y2,Z2,AA2,AB2,AC2-5)/30 * 100,0)</f>
         <v>30</v>
       </c>
       <c r="AN2" s="7">
-        <f t="shared" ref="AN2:AN52" si="5">ROUND(SUM((8-AD2),AE2,AF2,AG2,AH2-5)/30 * 100,0)</f>
+        <f t="shared" ref="AN2:AN57" si="5">ROUND(SUM((8-AD2),AE2,AF2,AG2,AH2-5)/30 * 100,0)</f>
         <v>43</v>
       </c>
       <c r="AO2" s="7"/>
       <c r="AP2" s="8">
-        <f t="shared" ref="AP2:AP44" si="6">ROW()</f>
+        <f t="shared" ref="AP2:AP57" si="6">ROW()</f>
         <v>2</v>
       </c>
     </row>
@@ -6594,6 +6636,10 @@
         <f t="shared" si="5"/>
         <v>37</v>
       </c>
+      <c r="AP45" s="8">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="5">
@@ -6718,6 +6764,10 @@
         <f t="shared" si="5"/>
         <v>53</v>
       </c>
+      <c r="AP46" s="8">
+        <f t="shared" si="6"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5">
@@ -6842,6 +6892,10 @@
         <f t="shared" si="5"/>
         <v>73</v>
       </c>
+      <c r="AP47" s="8">
+        <f t="shared" si="6"/>
+        <v>47</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="5">
@@ -6966,6 +7020,10 @@
         <f t="shared" si="5"/>
         <v>23</v>
       </c>
+      <c r="AP48" s="8">
+        <f t="shared" si="6"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="5">
@@ -7090,6 +7148,10 @@
         <f t="shared" si="5"/>
         <v>27</v>
       </c>
+      <c r="AP49" s="8">
+        <f t="shared" si="6"/>
+        <v>49</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="5">
@@ -7214,6 +7276,10 @@
         <f t="shared" si="5"/>
         <v>73</v>
       </c>
+      <c r="AP50" s="8">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="5">
@@ -7338,6 +7404,10 @@
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
+      <c r="AP51" s="8">
+        <f t="shared" si="6"/>
+        <v>51</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="5">
@@ -7462,6 +7532,10 @@
         <f t="shared" si="5"/>
         <v>53</v>
       </c>
+      <c r="AP52" s="8">
+        <f t="shared" si="6"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5">
@@ -7566,46 +7640,550 @@
       <c r="AH53" s="6">
         <v>5.0</v>
       </c>
+      <c r="AJ53" s="7">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="AK53" s="7">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="AL53" s="7">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="AM53" s="7">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="AN53" s="7">
+        <f t="shared" si="5"/>
+        <v>43</v>
+      </c>
+      <c r="AP53" s="8">
+        <f t="shared" si="6"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="54">
-      <c r="F54" s="2"/>
-      <c r="AJ54" s="7"/>
-      <c r="AK54" s="7"/>
-      <c r="AL54" s="7"/>
-      <c r="AM54" s="7"/>
-      <c r="AN54" s="7"/>
+      <c r="A54" s="5">
+        <v>44355.964501180555</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E54" s="6">
+        <v>21.0</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J54" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="K54" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="L54" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="M54" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="N54" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="O54" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="P54" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="Q54" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="R54" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="S54" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="T54" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="U54" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="V54" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="W54" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="X54" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="Y54" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="Z54" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="AA54" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="AB54" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="AC54" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="AD54" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="AE54" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="AF54" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="AG54" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="AH54" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="AJ54" s="7">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="AK54" s="7">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="AL54" s="7">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="AM54" s="7">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="AN54" s="7">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="AP54" s="8">
+        <f t="shared" si="6"/>
+        <v>54</v>
+      </c>
     </row>
     <row r="55">
-      <c r="F55" s="2"/>
-      <c r="AJ55" s="7"/>
-      <c r="AK55" s="7"/>
-      <c r="AL55" s="7"/>
-      <c r="AM55" s="7"/>
-      <c r="AN55" s="7"/>
+      <c r="A55" s="5">
+        <v>44356.36640221065</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E55" s="6">
+        <v>22.0</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J55" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="K55" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="L55" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="M55" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="N55" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="O55" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="P55" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="Q55" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="R55" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="S55" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="T55" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="U55" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="V55" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="W55" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="X55" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="Y55" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="Z55" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="AA55" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="AB55" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="AC55" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="AD55" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="AE55" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="AF55" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="AG55" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="AH55" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="AJ55" s="7">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="AK55" s="7">
+        <f t="shared" si="2"/>
+        <v>77</v>
+      </c>
+      <c r="AL55" s="7">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+      <c r="AM55" s="7">
+        <f t="shared" si="4"/>
+        <v>67</v>
+      </c>
+      <c r="AN55" s="7">
+        <f t="shared" si="5"/>
+        <v>77</v>
+      </c>
+      <c r="AP55" s="8">
+        <f t="shared" si="6"/>
+        <v>55</v>
+      </c>
     </row>
     <row r="56">
-      <c r="F56" s="2"/>
-      <c r="AJ56" s="7"/>
-      <c r="AK56" s="7"/>
-      <c r="AL56" s="7"/>
-      <c r="AM56" s="7"/>
-      <c r="AN56" s="7"/>
+      <c r="A56" s="5">
+        <v>44356.65908712963</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E56" s="6">
+        <v>19.0</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J56" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="K56" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="L56" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="M56" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="N56" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="O56" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="P56" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="Q56" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="R56" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="S56" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="T56" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="U56" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="V56" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="W56" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="X56" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="Y56" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="Z56" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="AA56" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="AB56" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="AC56" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="AD56" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="AE56" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="AF56" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="AG56" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="AH56" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="AJ56" s="7">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="AK56" s="7">
+        <f t="shared" si="2"/>
+        <v>97</v>
+      </c>
+      <c r="AL56" s="7">
+        <f t="shared" si="3"/>
+        <v>83</v>
+      </c>
+      <c r="AM56" s="7">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="AN56" s="7">
+        <f t="shared" si="5"/>
+        <v>73</v>
+      </c>
+      <c r="AP56" s="8">
+        <f t="shared" si="6"/>
+        <v>56</v>
+      </c>
     </row>
     <row r="57">
-      <c r="F57" s="2"/>
-      <c r="AJ57" s="7"/>
-      <c r="AK57" s="7"/>
-      <c r="AL57" s="7"/>
-      <c r="AM57" s="7"/>
-      <c r="AN57" s="7"/>
+      <c r="A57" s="5">
+        <v>44356.68013502315</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E57" s="6">
+        <v>22.0</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J57" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="K57" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="L57" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="M57" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="N57" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="O57" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="P57" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="Q57" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="R57" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="S57" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="T57" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="U57" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="V57" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="W57" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="X57" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="Y57" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="Z57" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="AA57" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="AB57" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="AC57" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="AD57" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="AE57" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="AF57" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="AG57" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="AH57" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="AJ57" s="7">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="AK57" s="7">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="AL57" s="7">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+      <c r="AM57" s="7">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="AN57" s="7">
+        <f t="shared" si="5"/>
+        <v>83</v>
+      </c>
+      <c r="AP57" s="8">
+        <f t="shared" si="6"/>
+        <v>57</v>
+      </c>
     </row>
     <row r="58">
       <c r="F58" s="2"/>
-      <c r="AJ58" s="7"/>
-      <c r="AK58" s="7"/>
-      <c r="AL58" s="7"/>
-      <c r="AM58" s="7"/>
-      <c r="AN58" s="7"/>
+      <c r="AJ58" s="10"/>
+      <c r="AK58" s="10"/>
+      <c r="AL58" s="10"/>
+      <c r="AM58" s="10"/>
+      <c r="AN58" s="10"/>
     </row>
     <row r="59">
       <c r="F59" s="2"/>
@@ -7641,15 +8219,35 @@
     </row>
     <row r="63">
       <c r="F63" s="2"/>
+      <c r="AJ63" s="7"/>
+      <c r="AK63" s="7"/>
+      <c r="AL63" s="7"/>
+      <c r="AM63" s="7"/>
+      <c r="AN63" s="7"/>
     </row>
     <row r="64">
       <c r="F64" s="2"/>
+      <c r="AJ64" s="7"/>
+      <c r="AK64" s="7"/>
+      <c r="AL64" s="7"/>
+      <c r="AM64" s="7"/>
+      <c r="AN64" s="7"/>
     </row>
     <row r="65">
       <c r="F65" s="2"/>
+      <c r="AJ65" s="7"/>
+      <c r="AK65" s="7"/>
+      <c r="AL65" s="7"/>
+      <c r="AM65" s="7"/>
+      <c r="AN65" s="7"/>
     </row>
     <row r="66">
       <c r="F66" s="2"/>
+      <c r="AJ66" s="7"/>
+      <c r="AK66" s="7"/>
+      <c r="AL66" s="7"/>
+      <c r="AM66" s="7"/>
+      <c r="AN66" s="7"/>
     </row>
     <row r="67">
       <c r="F67" s="2"/>
@@ -7911,6 +8509,18 @@
     </row>
     <row r="153">
       <c r="F153" s="2"/>
+    </row>
+    <row r="154">
+      <c r="F154" s="2"/>
+    </row>
+    <row r="155">
+      <c r="F155" s="2"/>
+    </row>
+    <row r="156">
+      <c r="F156" s="2"/>
+    </row>
+    <row r="157">
+      <c r="F157" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>